<commit_message>
Update C4E_Avanade.xlsx removing OPTIONAL fields
</commit_message>
<xml_diff>
--- a/resources/excel/C4E_Avanade.xlsx
+++ b/resources/excel/C4E_Avanade.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="179">
   <si>
     <t>Activity Title</t>
   </si>
@@ -91,9 +91,6 @@
     <t>30 young people directly enabled through a 12 week Entrepreneur program run by Flaare.
 Client DataBricks also participated as volunteers and loved it.
 An additional 6400 Enabled as a result of 8 youth workers attending one session of planning with Avanade which helped them to enable 20% more young people through strategic ideas.  20% of 4000 is 800 x 8 youth workers is 6400</t>
-  </si>
-  <si>
-    <t>OPTIONAL</t>
   </si>
   <si>
     <t>United Kingdom</t>
@@ -1064,20 +1061,14 @@
       <c r="E2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K2" s="7">
         <v>45546.89709490741</v>
@@ -1086,10 +1077,10 @@
         <v>45546.89709490741</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O2" s="8">
         <v>51.507351</v>
@@ -1097,9 +1088,7 @@
       <c r="P2" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q2" s="3"/>
       <c r="R2" s="9"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
@@ -1112,34 +1101,28 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K3" s="7">
         <v>45546.89709490741</v>
@@ -1148,10 +1131,10 @@
         <v>45546.89709490741</v>
       </c>
       <c r="M3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O3" s="8">
         <v>52.132633</v>
@@ -1159,9 +1142,7 @@
       <c r="P3" s="8">
         <v>5.291266</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
@@ -1174,34 +1155,28 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="7">
         <v>45449.897002314814</v>
@@ -1210,10 +1185,10 @@
         <v>45449.897002314814</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O4" s="8">
         <v>60.472023</v>
@@ -1221,9 +1196,7 @@
       <c r="P4" s="8">
         <v>8.468946</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
@@ -1236,34 +1209,28 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5" s="7">
         <v>45546.89699074074</v>
@@ -1272,10 +1239,10 @@
         <v>45546.89699074074</v>
       </c>
       <c r="M5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O5" s="8">
         <v>60.472023</v>
@@ -1283,9 +1250,7 @@
       <c r="P5" s="8">
         <v>8.468946</v>
       </c>
-      <c r="Q5" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -1298,34 +1263,28 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="7">
         <v>45546.89696759259</v>
@@ -1334,10 +1293,10 @@
         <v>45546.89696759259</v>
       </c>
       <c r="M6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O6" s="8">
         <v>60.472023</v>
@@ -1345,9 +1304,7 @@
       <c r="P6" s="8">
         <v>8.468946</v>
       </c>
-      <c r="Q6" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -1360,32 +1317,26 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I7" s="3"/>
       <c r="J7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K7" s="7">
         <v>45546.8969212963</v>
@@ -1394,10 +1345,10 @@
         <v>45546.8969212963</v>
       </c>
       <c r="M7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O7" s="8">
         <v>53.41291</v>
@@ -1405,9 +1356,7 @@
       <c r="P7" s="8">
         <v>-8.24389</v>
       </c>
-      <c r="Q7" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -1420,34 +1369,28 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="3"/>
+      <c r="J8" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K8" s="7">
         <v>45546.89690972222</v>
@@ -1456,10 +1399,10 @@
         <v>45546.89690972222</v>
       </c>
       <c r="M8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O8" s="8">
         <v>51.507351</v>
@@ -1467,9 +1410,7 @@
       <c r="P8" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q8" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -1482,34 +1423,28 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="3"/>
+      <c r="J9" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K9" s="7">
         <v>45546.896886574075</v>
@@ -1518,10 +1453,10 @@
         <v>45546.896886574075</v>
       </c>
       <c r="M9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O9" s="8">
         <v>51.507351</v>
@@ -1529,9 +1464,7 @@
       <c r="P9" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q9" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -1544,46 +1477,40 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="3"/>
+      <c r="J10" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K10" s="7">
         <v>45607.896875</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O10" s="8">
         <v>51.507351</v>
@@ -1591,9 +1518,7 @@
       <c r="P10" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -1606,34 +1531,28 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K11" s="7">
         <v>45546.89601851852</v>
@@ -1642,10 +1561,10 @@
         <v>45546.89601851852</v>
       </c>
       <c r="M11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O11" s="8">
         <v>53.41291</v>
@@ -1653,9 +1572,7 @@
       <c r="P11" s="8">
         <v>-8.24389</v>
       </c>
-      <c r="Q11" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -1668,34 +1585,28 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I12" s="3"/>
       <c r="J12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K12" s="7">
         <v>45546.89596064815</v>
@@ -1704,10 +1615,10 @@
         <v>45546.89596064815</v>
       </c>
       <c r="M12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O12" s="8">
         <v>47.59397</v>
@@ -1715,9 +1626,7 @@
       <c r="P12" s="8">
         <v>14.12456</v>
       </c>
-      <c r="Q12" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -1730,46 +1639,40 @@
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="6" t="s">
+      <c r="L13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="M13" s="6" t="s">
+      <c r="N13" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O13" s="8">
         <v>51.507351</v>
@@ -1777,9 +1680,7 @@
       <c r="P13" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q13" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -1792,46 +1693,40 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="6" t="s">
+      <c r="L14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="M14" s="6" t="s">
+      <c r="N14" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O14" s="8">
         <v>51.507351</v>
@@ -1839,9 +1734,7 @@
       <c r="P14" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q14" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -1854,34 +1747,28 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="C15" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I15" s="3"/>
       <c r="J15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K15" s="10">
         <v>45608.0</v>
@@ -1890,10 +1777,10 @@
         <v>45608.0</v>
       </c>
       <c r="M15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O15" s="8">
         <v>39.3260685</v>
@@ -1901,9 +1788,7 @@
       <c r="P15" s="8">
         <v>-4.8379791</v>
       </c>
-      <c r="Q15" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -1916,34 +1801,28 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I16" s="3"/>
       <c r="J16" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K16" s="10">
         <v>45608.0</v>
@@ -1952,10 +1831,10 @@
         <v>45608.0</v>
       </c>
       <c r="M16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O16" s="8">
         <v>39.6621648</v>
@@ -1963,9 +1842,7 @@
       <c r="P16" s="8">
         <v>-8.1353519</v>
       </c>
-      <c r="Q16" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -1978,34 +1855,28 @@
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="I17" s="3"/>
       <c r="J17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17" s="10">
         <v>45608.0</v>
@@ -2014,10 +1885,10 @@
         <v>45608.0</v>
       </c>
       <c r="M17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O17" s="8">
         <v>47.59397</v>
@@ -2025,9 +1896,7 @@
       <c r="P17" s="8">
         <v>14.12456</v>
       </c>
-      <c r="Q17" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
@@ -2040,34 +1909,28 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="4" t="s">
+      <c r="I18" s="3"/>
+      <c r="J18" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K18" s="10">
         <v>45608.0</v>
@@ -2076,10 +1939,10 @@
         <v>45608.0</v>
       </c>
       <c r="M18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O18" s="8">
         <v>51.507351</v>
@@ -2087,9 +1950,7 @@
       <c r="P18" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q18" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
@@ -2102,34 +1963,28 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="I19" s="3"/>
       <c r="J19" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K19" s="10">
         <v>45608.0</v>
@@ -2138,10 +1993,10 @@
         <v>45608.0</v>
       </c>
       <c r="M19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O19" s="8">
         <v>47.59397</v>
@@ -2149,9 +2004,7 @@
       <c r="P19" s="8">
         <v>14.12456</v>
       </c>
-      <c r="Q19" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
@@ -2164,34 +2017,28 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="C20" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I20" s="3"/>
       <c r="J20" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K20" s="10">
         <v>45608.0</v>
@@ -2200,10 +2047,10 @@
         <v>45608.0</v>
       </c>
       <c r="M20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N20" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O20" s="8">
         <v>42.6384261</v>
@@ -2211,9 +2058,7 @@
       <c r="P20" s="8">
         <v>12.674297</v>
       </c>
-      <c r="Q20" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
@@ -2226,34 +2071,28 @@
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="I21" s="3"/>
       <c r="J21" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K21" s="10">
         <v>45608.0</v>
@@ -2262,10 +2101,10 @@
         <v>45608.0</v>
       </c>
       <c r="M21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N21" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O21" s="8">
         <v>39.6621648</v>
@@ -2273,9 +2112,7 @@
       <c r="P21" s="8">
         <v>-8.1353519</v>
       </c>
-      <c r="Q21" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -2288,34 +2125,28 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="C22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I22" s="3"/>
       <c r="J22" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K22" s="10">
         <v>45608.0</v>
@@ -2324,10 +2155,10 @@
         <v>45608.0</v>
       </c>
       <c r="M22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N22" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O22" s="8">
         <v>52.215933</v>
@@ -2335,9 +2166,7 @@
       <c r="P22" s="8">
         <v>19.134422</v>
       </c>
-      <c r="Q22" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
@@ -2350,34 +2179,28 @@
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="I23" s="3"/>
       <c r="J23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K23" s="10">
         <v>45608.0</v>
@@ -2386,10 +2209,10 @@
         <v>45608.0</v>
       </c>
       <c r="M23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N23" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O23" s="8">
         <v>52.215933</v>
@@ -2397,9 +2220,7 @@
       <c r="P23" s="8">
         <v>19.134422</v>
       </c>
-      <c r="Q23" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
@@ -2412,34 +2233,28 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="4" t="s">
+      <c r="I24" s="3"/>
+      <c r="J24" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K24" s="10">
         <v>45608.0</v>
@@ -2448,10 +2263,10 @@
         <v>45608.0</v>
       </c>
       <c r="M24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N24" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O24" s="8">
         <v>51.507351</v>
@@ -2459,9 +2274,7 @@
       <c r="P24" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q24" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -2474,34 +2287,28 @@
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="4" t="s">
+      <c r="I25" s="3"/>
+      <c r="J25" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K25" s="10">
         <v>45608.0</v>
@@ -2510,10 +2317,10 @@
         <v>45608.0</v>
       </c>
       <c r="M25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O25" s="8">
         <v>51.507351</v>
@@ -2521,9 +2328,7 @@
       <c r="P25" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q25" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -2536,34 +2341,28 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="C26" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="I26" s="3"/>
       <c r="J26" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K26" s="10">
         <v>45608.0</v>
@@ -2572,10 +2371,10 @@
         <v>45608.0</v>
       </c>
       <c r="M26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N26" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O26" s="8">
         <v>52.215933</v>
@@ -2583,9 +2382,7 @@
       <c r="P26" s="8">
         <v>19.134422</v>
       </c>
-      <c r="Q26" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
@@ -2598,32 +2395,26 @@
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I27" s="3"/>
       <c r="J27" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K27" s="10">
         <v>45608.0</v>
@@ -2632,10 +2423,10 @@
         <v>45608.0</v>
       </c>
       <c r="M27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O27" s="8">
         <v>46.7985624</v>
@@ -2643,9 +2434,7 @@
       <c r="P27" s="8">
         <v>8.2319736</v>
       </c>
-      <c r="Q27" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
@@ -2658,34 +2447,28 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="4" t="s">
+      <c r="I28" s="3"/>
+      <c r="J28" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K28" s="10">
         <v>45608.0</v>
@@ -2694,10 +2477,10 @@
         <v>45608.0</v>
       </c>
       <c r="M28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O28" s="8">
         <v>51.507351</v>
@@ -2705,9 +2488,7 @@
       <c r="P28" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q28" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
@@ -2720,34 +2501,28 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="4" t="s">
+      <c r="I29" s="3"/>
+      <c r="J29" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K29" s="10">
         <v>45608.0</v>
@@ -2756,10 +2531,10 @@
         <v>45608.0</v>
       </c>
       <c r="M29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N29" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O29" s="8">
         <v>51.507351</v>
@@ -2767,9 +2542,7 @@
       <c r="P29" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q29" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
@@ -2782,34 +2555,28 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="C30" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F30" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="4" t="s">
+      <c r="I30" s="3"/>
+      <c r="J30" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K30" s="10">
         <v>45608.0</v>
@@ -2818,10 +2585,10 @@
         <v>45608.0</v>
       </c>
       <c r="M30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O30" s="8">
         <v>51.507351</v>
@@ -2829,9 +2596,7 @@
       <c r="P30" s="8">
         <v>-0.127758</v>
       </c>
-      <c r="Q30" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
@@ -2844,34 +2609,28 @@
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>128</v>
-      </c>
       <c r="C31" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="I31" s="3"/>
       <c r="J31" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K31" s="10">
         <v>45608.0</v>
@@ -2880,10 +2639,10 @@
         <v>45608.0</v>
       </c>
       <c r="M31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N31" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O31" s="8">
         <v>51.1638175</v>
@@ -2891,9 +2650,7 @@
       <c r="P31" s="8">
         <v>10.4478313</v>
       </c>
-      <c r="Q31" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
@@ -2906,34 +2663,28 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="C32" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="I32" s="3"/>
       <c r="J32" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K32" s="10">
         <v>45608.0</v>
@@ -2942,10 +2693,10 @@
         <v>45608.0</v>
       </c>
       <c r="M32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O32" s="8">
         <v>47.59397</v>
@@ -2953,9 +2704,7 @@
       <c r="P32" s="8">
         <v>14.12456</v>
       </c>
-      <c r="Q32" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -2968,34 +2717,28 @@
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="I33" s="3"/>
       <c r="J33" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K33" s="10">
         <v>45608.0</v>
@@ -3004,10 +2747,10 @@
         <v>45608.0</v>
       </c>
       <c r="M33" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N33" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N33" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O33" s="8">
         <v>52.215933</v>
@@ -3015,9 +2758,7 @@
       <c r="P33" s="8">
         <v>19.134422</v>
       </c>
-      <c r="Q33" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
@@ -3030,34 +2771,28 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
       <c r="H34" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="I34" s="3"/>
       <c r="J34" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K34" s="10">
         <v>45608.0</v>
@@ -3066,10 +2801,10 @@
         <v>45608.0</v>
       </c>
       <c r="M34" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N34" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O34" s="8">
         <v>52.215933</v>
@@ -3077,9 +2812,7 @@
       <c r="P34" s="8">
         <v>19.134422</v>
       </c>
-      <c r="Q34" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -3092,34 +2825,28 @@
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="C35" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
       <c r="H35" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="I35" s="3"/>
       <c r="J35" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K35" s="10">
         <v>45608.0</v>
@@ -3128,10 +2855,10 @@
         <v>45608.0</v>
       </c>
       <c r="M35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N35" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="O35" s="8">
         <v>52.215933</v>
@@ -3139,9 +2866,7 @@
       <c r="P35" s="8">
         <v>19.134422</v>
       </c>
-      <c r="Q35" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
@@ -30196,32 +29921,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7"/>
@@ -30263,10 +29988,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2">
@@ -30274,7 +29999,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3">
@@ -30282,7 +30007,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4">
@@ -30290,7 +30015,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5">
@@ -30298,7 +30023,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6">
@@ -30306,7 +30031,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
@@ -30314,7 +30039,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8">
@@ -30322,7 +30047,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9">
@@ -30330,7 +30055,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
@@ -30338,7 +30063,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11"/>
@@ -30376,10 +30101,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2">
@@ -30387,7 +30112,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3">
@@ -30395,7 +30120,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4">
@@ -30403,7 +30128,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5">
@@ -30411,7 +30136,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6">
@@ -30419,7 +30144,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7">
@@ -30427,7 +30152,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8">
@@ -30435,7 +30160,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9">
@@ -30443,7 +30168,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
@@ -30451,7 +30176,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11">
@@ -30459,7 +30184,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12">
@@ -30467,10 +30192,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="13">
@@ -30478,7 +30203,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14">
@@ -30486,7 +30211,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
@@ -30494,7 +30219,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16">
@@ -30502,7 +30227,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17">
@@ -30510,7 +30235,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18">
@@ -30518,7 +30243,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19">
@@ -30526,7 +30251,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20">
@@ -30534,7 +30259,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -30560,27 +30285,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6"/>

</xml_diff>

<commit_message>
Update C4E_Avanade.xlsx fix longitude latitude
</commit_message>
<xml_diff>
--- a/resources/excel/C4E_Avanade.xlsx
+++ b/resources/excel/C4E_Avanade.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="177">
   <si>
     <t>Activity Title</t>
   </si>
@@ -94,12 +94,6 @@
   </si>
   <si>
     <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>Not mandatory if the event is online</t>
-  </si>
-  <si>
-    <t>Mandatory if the activity type in open online</t>
   </si>
   <si>
     <t>kirsty.christie@avanade.com</t>
@@ -706,7 +700,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
@@ -1067,26 +1061,22 @@
         <v>23</v>
       </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J2" s="6"/>
       <c r="K2" s="7">
         <v>45546.89709490741</v>
       </c>
       <c r="L2" s="7">
         <v>45546.89709490741</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M2" s="6"/>
       <c r="N2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O2" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P2" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P2" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="9"/>
@@ -1101,46 +1091,42 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="J3" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J3" s="6"/>
       <c r="K3" s="7">
         <v>45546.89709490741</v>
       </c>
       <c r="L3" s="7">
         <v>45546.89709490741</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M3" s="6"/>
       <c r="N3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O3" s="8">
+        <v>5.291266</v>
+      </c>
+      <c r="P3" s="8">
         <v>52.132633</v>
-      </c>
-      <c r="P3" s="8">
-        <v>5.291266</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -1155,46 +1141,42 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J4" s="6"/>
       <c r="K4" s="7">
         <v>45449.897002314814</v>
       </c>
       <c r="L4" s="7">
         <v>45449.897002314814</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M4" s="6"/>
       <c r="N4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O4" s="8">
+        <v>8.468946</v>
+      </c>
+      <c r="P4" s="8">
         <v>60.472023</v>
-      </c>
-      <c r="P4" s="8">
-        <v>8.468946</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -1209,46 +1191,42 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J5" s="6"/>
       <c r="K5" s="7">
         <v>45546.89699074074</v>
       </c>
       <c r="L5" s="7">
         <v>45546.89699074074</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M5" s="6"/>
       <c r="N5" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O5" s="8">
+        <v>8.468946</v>
+      </c>
+      <c r="P5" s="8">
         <v>60.472023</v>
-      </c>
-      <c r="P5" s="8">
-        <v>8.468946</v>
       </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
@@ -1263,46 +1241,42 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J6" s="6"/>
       <c r="K6" s="7">
         <v>45546.89696759259</v>
       </c>
       <c r="L6" s="7">
         <v>45546.89696759259</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M6" s="6"/>
       <c r="N6" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O6" s="8">
+        <v>8.468946</v>
+      </c>
+      <c r="P6" s="8">
         <v>60.472023</v>
-      </c>
-      <c r="P6" s="8">
-        <v>8.468946</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -1317,44 +1291,40 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J7" s="6"/>
       <c r="K7" s="7">
         <v>45546.8969212963</v>
       </c>
       <c r="L7" s="7">
         <v>45546.8969212963</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M7" s="6"/>
       <c r="N7" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O7" s="8">
+        <v>-8.24389</v>
+      </c>
+      <c r="P7" s="8">
         <v>53.41291</v>
-      </c>
-      <c r="P7" s="8">
-        <v>-8.24389</v>
       </c>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -1369,19 +1339,19 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1389,26 +1359,22 @@
         <v>23</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J8" s="6"/>
       <c r="K8" s="7">
         <v>45546.89690972222</v>
       </c>
       <c r="L8" s="7">
         <v>45546.89690972222</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M8" s="6"/>
       <c r="N8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O8" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P8" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P8" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
@@ -1423,19 +1389,19 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1443,26 +1409,22 @@
         <v>23</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J9" s="6"/>
       <c r="K9" s="7">
         <v>45546.896886574075</v>
       </c>
       <c r="L9" s="7">
         <v>45546.896886574075</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M9" s="6"/>
       <c r="N9" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O9" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P9" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P9" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
@@ -1477,19 +1439,19 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1497,26 +1459,22 @@
         <v>23</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J10" s="6"/>
       <c r="K10" s="7">
         <v>45607.896875</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>25</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="M10" s="6"/>
       <c r="N10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O10" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P10" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P10" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
@@ -1531,46 +1489,42 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J11" s="6"/>
       <c r="K11" s="7">
         <v>45546.89601851852</v>
       </c>
       <c r="L11" s="7">
         <v>45546.89601851852</v>
       </c>
-      <c r="M11" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M11" s="6"/>
       <c r="N11" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O11" s="8">
+        <v>-8.24389</v>
+      </c>
+      <c r="P11" s="8">
         <v>53.41291</v>
-      </c>
-      <c r="P11" s="8">
-        <v>-8.24389</v>
       </c>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
@@ -1585,46 +1539,42 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J12" s="6"/>
       <c r="K12" s="7">
         <v>45546.89596064815</v>
       </c>
       <c r="L12" s="7">
         <v>45546.89596064815</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M12" s="6"/>
       <c r="N12" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O12" s="8">
+        <v>14.12456</v>
+      </c>
+      <c r="P12" s="8">
         <v>47.59397</v>
-      </c>
-      <c r="P12" s="8">
-        <v>14.12456</v>
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
@@ -1639,19 +1589,19 @@
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1659,26 +1609,22 @@
         <v>23</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="6"/>
+      <c r="K13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="O13" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P13" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P13" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
@@ -1693,19 +1639,19 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1713,26 +1659,22 @@
         <v>23</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="6"/>
+      <c r="K14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="6"/>
+      <c r="N14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="O14" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P14" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P14" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
@@ -1747,46 +1689,42 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J15" s="6"/>
       <c r="K15" s="10">
         <v>45608.0</v>
       </c>
       <c r="L15" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M15" s="6"/>
       <c r="N15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O15" s="8">
+        <v>-4.8379791</v>
+      </c>
+      <c r="P15" s="8">
         <v>39.3260685</v>
-      </c>
-      <c r="P15" s="8">
-        <v>-4.8379791</v>
       </c>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
@@ -1801,46 +1739,42 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J16" s="6"/>
       <c r="K16" s="10">
         <v>45608.0</v>
       </c>
       <c r="L16" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M16" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M16" s="6"/>
       <c r="N16" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O16" s="8">
+        <v>-8.1353519</v>
+      </c>
+      <c r="P16" s="8">
         <v>39.6621648</v>
-      </c>
-      <c r="P16" s="8">
-        <v>-8.1353519</v>
       </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
@@ -1855,46 +1789,42 @@
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J17" s="6"/>
       <c r="K17" s="10">
         <v>45608.0</v>
       </c>
       <c r="L17" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M17" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M17" s="6"/>
       <c r="N17" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O17" s="8">
+        <v>14.12456</v>
+      </c>
+      <c r="P17" s="8">
         <v>47.59397</v>
-      </c>
-      <c r="P17" s="8">
-        <v>14.12456</v>
       </c>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
@@ -1909,19 +1839,19 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1929,26 +1859,22 @@
         <v>23</v>
       </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J18" s="6"/>
       <c r="K18" s="10">
         <v>45608.0</v>
       </c>
       <c r="L18" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M18" s="6"/>
       <c r="N18" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O18" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P18" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P18" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
@@ -1963,46 +1889,42 @@
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J19" s="6"/>
       <c r="K19" s="10">
         <v>45608.0</v>
       </c>
       <c r="L19" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M19" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M19" s="6"/>
       <c r="N19" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O19" s="8">
+        <v>14.12456</v>
+      </c>
+      <c r="P19" s="8">
         <v>47.59397</v>
-      </c>
-      <c r="P19" s="8">
-        <v>14.12456</v>
       </c>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
@@ -2017,46 +1939,42 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J20" s="6"/>
       <c r="K20" s="10">
         <v>45608.0</v>
       </c>
       <c r="L20" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M20" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M20" s="6"/>
       <c r="N20" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O20" s="8">
+        <v>12.674297</v>
+      </c>
+      <c r="P20" s="8">
         <v>42.6384261</v>
-      </c>
-      <c r="P20" s="8">
-        <v>12.674297</v>
       </c>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
@@ -2071,46 +1989,42 @@
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J21" s="6"/>
       <c r="K21" s="10">
         <v>45608.0</v>
       </c>
       <c r="L21" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M21" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M21" s="6"/>
       <c r="N21" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O21" s="8">
+        <v>-8.1353519</v>
+      </c>
+      <c r="P21" s="8">
         <v>39.6621648</v>
-      </c>
-      <c r="P21" s="8">
-        <v>-8.1353519</v>
       </c>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
@@ -2125,46 +2039,42 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="J22" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J22" s="6"/>
       <c r="K22" s="10">
         <v>45608.0</v>
       </c>
       <c r="L22" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M22" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M22" s="6"/>
       <c r="N22" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O22" s="8">
+        <v>19.134422</v>
+      </c>
+      <c r="P22" s="8">
         <v>52.215933</v>
-      </c>
-      <c r="P22" s="8">
-        <v>19.134422</v>
       </c>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
@@ -2179,46 +2089,42 @@
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J23" s="6"/>
       <c r="K23" s="10">
         <v>45608.0</v>
       </c>
       <c r="L23" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M23" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M23" s="6"/>
       <c r="N23" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O23" s="8">
+        <v>19.134422</v>
+      </c>
+      <c r="P23" s="8">
         <v>52.215933</v>
-      </c>
-      <c r="P23" s="8">
-        <v>19.134422</v>
       </c>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
@@ -2233,19 +2139,19 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="E24" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -2253,26 +2159,22 @@
         <v>23</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J24" s="6"/>
       <c r="K24" s="10">
         <v>45608.0</v>
       </c>
       <c r="L24" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M24" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M24" s="6"/>
       <c r="N24" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O24" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P24" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P24" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
@@ -2287,19 +2189,19 @@
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -2307,26 +2209,22 @@
         <v>23</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J25" s="6"/>
       <c r="K25" s="10">
         <v>45608.0</v>
       </c>
       <c r="L25" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M25" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M25" s="6"/>
       <c r="N25" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O25" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P25" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P25" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
@@ -2341,46 +2239,42 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I26" s="3"/>
-      <c r="J26" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J26" s="6"/>
       <c r="K26" s="10">
         <v>45608.0</v>
       </c>
       <c r="L26" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M26" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M26" s="6"/>
       <c r="N26" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O26" s="8">
+        <v>19.134422</v>
+      </c>
+      <c r="P26" s="8">
         <v>52.215933</v>
-      </c>
-      <c r="P26" s="8">
-        <v>19.134422</v>
       </c>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
@@ -2395,44 +2289,40 @@
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I27" s="3"/>
-      <c r="J27" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J27" s="6"/>
       <c r="K27" s="10">
         <v>45608.0</v>
       </c>
       <c r="L27" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M27" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M27" s="6"/>
       <c r="N27" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O27" s="8">
+        <v>8.2319736</v>
+      </c>
+      <c r="P27" s="8">
         <v>46.7985624</v>
-      </c>
-      <c r="P27" s="8">
-        <v>8.2319736</v>
       </c>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
@@ -2447,19 +2337,19 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="E28" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -2467,26 +2357,22 @@
         <v>23</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J28" s="6"/>
       <c r="K28" s="10">
         <v>45608.0</v>
       </c>
       <c r="L28" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M28" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M28" s="6"/>
       <c r="N28" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O28" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P28" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P28" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
@@ -2501,19 +2387,19 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -2521,26 +2407,22 @@
         <v>23</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J29" s="6"/>
       <c r="K29" s="10">
         <v>45608.0</v>
       </c>
       <c r="L29" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M29" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M29" s="6"/>
       <c r="N29" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O29" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P29" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P29" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
@@ -2555,19 +2437,19 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -2575,26 +2457,22 @@
         <v>23</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J30" s="6"/>
       <c r="K30" s="10">
         <v>45608.0</v>
       </c>
       <c r="L30" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M30" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M30" s="6"/>
       <c r="N30" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O30" s="8">
+        <v>-0.127758</v>
+      </c>
+      <c r="P30" s="8">
         <v>51.507351</v>
-      </c>
-      <c r="P30" s="8">
-        <v>-0.127758</v>
       </c>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
@@ -2609,46 +2487,42 @@
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I31" s="3"/>
-      <c r="J31" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J31" s="6"/>
       <c r="K31" s="10">
         <v>45608.0</v>
       </c>
       <c r="L31" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M31" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M31" s="6"/>
       <c r="N31" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O31" s="8">
+        <v>10.4478313</v>
+      </c>
+      <c r="P31" s="8">
         <v>51.1638175</v>
-      </c>
-      <c r="P31" s="8">
-        <v>10.4478313</v>
       </c>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
@@ -2663,46 +2537,42 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I32" s="3"/>
-      <c r="J32" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J32" s="6"/>
       <c r="K32" s="10">
         <v>45608.0</v>
       </c>
       <c r="L32" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M32" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M32" s="6"/>
       <c r="N32" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O32" s="8">
+        <v>14.12456</v>
+      </c>
+      <c r="P32" s="8">
         <v>47.59397</v>
-      </c>
-      <c r="P32" s="8">
-        <v>14.12456</v>
       </c>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
@@ -2717,46 +2587,42 @@
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I33" s="3"/>
-      <c r="J33" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J33" s="6"/>
       <c r="K33" s="10">
         <v>45608.0</v>
       </c>
       <c r="L33" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M33" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M33" s="6"/>
       <c r="N33" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O33" s="8">
+        <v>19.134422</v>
+      </c>
+      <c r="P33" s="8">
         <v>52.215933</v>
-      </c>
-      <c r="P33" s="8">
-        <v>19.134422</v>
       </c>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
@@ -2771,46 +2637,42 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I34" s="3"/>
-      <c r="J34" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J34" s="6"/>
       <c r="K34" s="10">
         <v>45608.0</v>
       </c>
       <c r="L34" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M34" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M34" s="6"/>
       <c r="N34" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O34" s="8">
+        <v>19.134422</v>
+      </c>
+      <c r="P34" s="8">
         <v>52.215933</v>
-      </c>
-      <c r="P34" s="8">
-        <v>19.134422</v>
       </c>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
@@ -2825,46 +2687,42 @@
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I35" s="3"/>
-      <c r="J35" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J35" s="6"/>
       <c r="K35" s="10">
         <v>45608.0</v>
       </c>
       <c r="L35" s="10">
         <v>45608.0</v>
       </c>
-      <c r="M35" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="M35" s="6"/>
       <c r="N35" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="O35" s="8">
+        <v>19.134422</v>
+      </c>
+      <c r="P35" s="8">
         <v>52.215933</v>
-      </c>
-      <c r="P35" s="8">
-        <v>19.134422</v>
       </c>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
@@ -29921,32 +29779,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7"/>
@@ -29988,10 +29846,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
@@ -29999,7 +29857,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3">
@@ -30007,7 +29865,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4">
@@ -30015,7 +29873,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
@@ -30023,7 +29881,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6">
@@ -30031,7 +29889,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7">
@@ -30039,7 +29897,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8">
@@ -30047,7 +29905,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9">
@@ -30055,7 +29913,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -30063,7 +29921,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11"/>
@@ -30101,10 +29959,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
@@ -30112,7 +29970,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3">
@@ -30120,7 +29978,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4">
@@ -30128,7 +29986,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5">
@@ -30136,7 +29994,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6">
@@ -30144,7 +30002,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7">
@@ -30152,7 +30010,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8">
@@ -30160,7 +30018,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9">
@@ -30168,7 +30026,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -30176,7 +30034,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11">
@@ -30184,7 +30042,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
@@ -30192,10 +30050,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
@@ -30203,7 +30061,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14">
@@ -30211,7 +30069,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15">
@@ -30219,7 +30077,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16">
@@ -30227,7 +30085,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17">
@@ -30235,7 +30093,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18">
@@ -30243,7 +30101,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19">
@@ -30251,7 +30109,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20">
@@ -30259,7 +30117,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -30285,27 +30143,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6"/>

</xml_diff>